<commit_message>
resetting titles after demo
</commit_message>
<xml_diff>
--- a/src/app/data/Database.xlsx
+++ b/src/app/data/Database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="7940" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="7940"/>
   </bookViews>
   <sheets>
     <sheet name="ISO" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3003" uniqueCount="1601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3001" uniqueCount="1599">
   <si>
     <t>id</t>
   </si>
@@ -5065,12 +5065,6 @@
   </si>
   <si>
     <t>Article(49)(5): In the absence of an adequacy decision, Union or Member State law may, for important reasons of public interest, expressly set limits to the...</t>
-  </si>
-  <si>
-    <t>5 - Section 5</t>
-  </si>
-  <si>
-    <t>5.2 - Section 5.2</t>
   </si>
 </sst>
 </file>
@@ -5115,9 +5109,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5460,8 +5457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5491,8 +5488,8 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>1599</v>
+      <c r="B2" s="2">
+        <v>5</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -5502,8 +5499,8 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>1600</v>
+      <c r="B3" s="2">
+        <v>5.2</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -7296,7 +7293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E406"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>